<commit_message>
circlefloatarray mit faktor 2 figur schliessen neu
report_HaALT neu: lokale Tastenfunktion

usb.swift: readtimer auf 0.5s
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4B4E78-48D8-A547-A510-518C34CAB213}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445299D2-E544-A64C-8896-957380107146}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="2880" windowWidth="26680" windowHeight="10500" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="12220" yWindow="24480" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
   <si>
     <t>schrittexA</t>
   </si>
@@ -137,13 +137,34 @@
   </si>
   <si>
     <t>position lage im Schnittpolygom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delayzC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">delayzD,  </t>
+  </si>
+  <si>
+    <t>sendbuffer</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>drillstaus</t>
+  </si>
+  <si>
+    <t>abschnittnummerH</t>
+  </si>
+  <si>
+    <t>abschnittnummerL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +199,13 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC41A16"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -219,6 +247,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1045,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C059D-FBB1-A24A-890C-2DC09AAA9BCC}">
-  <dimension ref="A1:AV26"/>
+  <dimension ref="A1:AV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,390 +1090,249 @@
     <col min="1" max="48" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" s="7" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:48" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" s="7" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>13</v>
+      </c>
+      <c r="O3">
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+      <c r="Q3">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <v>17</v>
+      </c>
+      <c r="S3">
+        <v>18</v>
+      </c>
+      <c r="T3">
+        <v>19</v>
+      </c>
+      <c r="U3">
+        <v>20</v>
+      </c>
+      <c r="V3">
+        <v>21</v>
+      </c>
+      <c r="W3">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X3">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y3">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z3">
+        <v>25</v>
+      </c>
+      <c r="AA3">
+        <v>26</v>
+      </c>
+      <c r="AB3">
+        <v>27</v>
+      </c>
+      <c r="AC3">
+        <v>28</v>
+      </c>
+      <c r="AD3">
+        <v>29</v>
+      </c>
+      <c r="AE3">
+        <v>30</v>
+      </c>
+      <c r="AF3">
+        <v>31</v>
+      </c>
+      <c r="AG3">
+        <v>32</v>
+      </c>
+      <c r="AH3">
+        <v>33</v>
+      </c>
+      <c r="AI3">
+        <v>34</v>
+      </c>
+      <c r="AJ3">
+        <v>35</v>
+      </c>
+      <c r="AK3">
         <v>36</v>
       </c>
-      <c r="AA1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>6</v>
-      </c>
-      <c r="H2">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
-      </c>
-      <c r="K2">
-        <v>10</v>
-      </c>
-      <c r="L2">
-        <v>11</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-      <c r="N2">
-        <v>13</v>
-      </c>
-      <c r="O2">
-        <v>14</v>
-      </c>
-      <c r="P2">
-        <v>15</v>
-      </c>
-      <c r="Q2">
-        <v>16</v>
-      </c>
-      <c r="R2">
-        <v>17</v>
-      </c>
-      <c r="S2">
-        <v>18</v>
-      </c>
-      <c r="T2">
-        <v>19</v>
-      </c>
-      <c r="U2">
-        <v>20</v>
-      </c>
-      <c r="V2">
-        <v>21</v>
-      </c>
-      <c r="W2">
-        <v>22</v>
-      </c>
-      <c r="X2">
-        <v>23</v>
-      </c>
-      <c r="Y2">
-        <v>24</v>
-      </c>
-      <c r="Z2">
-        <v>25</v>
-      </c>
-      <c r="AA2">
-        <v>26</v>
-      </c>
-      <c r="AB2">
-        <v>27</v>
-      </c>
-      <c r="AC2">
-        <v>28</v>
-      </c>
-      <c r="AD2">
-        <v>29</v>
-      </c>
-      <c r="AE2">
-        <v>30</v>
-      </c>
-      <c r="AF2">
-        <v>31</v>
-      </c>
-      <c r="AG2">
-        <v>32</v>
-      </c>
-      <c r="AH2">
-        <v>33</v>
-      </c>
-      <c r="AI2">
-        <v>34</v>
-      </c>
-      <c r="AJ2">
-        <v>35</v>
-      </c>
-      <c r="AK2">
-        <v>36</v>
-      </c>
-      <c r="AL2">
+      <c r="AL3">
         <v>37</v>
       </c>
-      <c r="AM2">
+      <c r="AM3">
         <v>38</v>
       </c>
-      <c r="AN2">
+      <c r="AN3">
         <v>39</v>
       </c>
-      <c r="AO2">
+      <c r="AO3">
         <v>40</v>
       </c>
-      <c r="AP2">
+      <c r="AP3">
         <v>41</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ3">
         <v>42</v>
       </c>
-      <c r="AR2">
+      <c r="AR3">
         <v>43</v>
       </c>
-      <c r="AS2">
+      <c r="AS3">
         <v>44</v>
       </c>
-      <c r="AT2">
+      <c r="AT3">
         <v>45</v>
       </c>
-      <c r="AU2">
+      <c r="AU3">
         <v>46</v>
       </c>
-      <c r="AV2">
+      <c r="AV3">
         <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>101</v>
-      </c>
-      <c r="B3" s="5">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>105</v>
-      </c>
-      <c r="J3" s="5">
-        <v>14</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>128</v>
-      </c>
-      <c r="M3" s="5">
-        <v>6</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>97</v>
-      </c>
-      <c r="P3" s="5">
-        <v>128</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-      <c r="R3" s="5">
-        <v>0</v>
-      </c>
-      <c r="S3" s="5">
-        <v>0</v>
-      </c>
-      <c r="T3" s="5">
-        <v>0</v>
-      </c>
-      <c r="U3" s="5">
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <v>0</v>
-      </c>
-      <c r="W3" s="5">
-        <v>0</v>
-      </c>
-      <c r="X3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="5">
-        <v>77</v>
-      </c>
-      <c r="AE3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="5">
-        <v>128</v>
-      </c>
-      <c r="AG3" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="5">
-        <v>255</v>
-      </c>
-      <c r="AM3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="5">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>194</v>
+        <v>101</v>
       </c>
       <c r="B4" s="5">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -1448,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
@@ -1460,28 +1353,28 @@
         <v>0</v>
       </c>
       <c r="I4" s="5">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="J4" s="5">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
       </c>
       <c r="L4" s="5">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="M4" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N4" s="5">
         <v>0</v>
       </c>
       <c r="O4" s="5">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="P4" s="5">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
@@ -1511,13 +1404,13 @@
         <v>0</v>
       </c>
       <c r="Z4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" s="5">
         <v>0</v>
       </c>
       <c r="AB4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="5">
         <v>2</v>
@@ -1582,10 +1475,10 @@
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="B5" s="5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5">
         <v>0</v>
@@ -1594,40 +1487,40 @@
         <v>0</v>
       </c>
       <c r="E5" s="5">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>101</v>
+      </c>
+      <c r="J5" s="5">
+        <v>9</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
         <v>7</v>
       </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>66</v>
-      </c>
-      <c r="J5" s="5">
-        <v>6</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>128</v>
-      </c>
-      <c r="M5" s="5">
-        <v>10</v>
-      </c>
       <c r="N5" s="5">
         <v>0</v>
       </c>
       <c r="O5" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P5" s="5">
-        <v>128</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="5">
         <v>0</v>
@@ -1663,10 +1556,10 @@
         <v>0</v>
       </c>
       <c r="AB5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="5">
         <v>2</v>
-      </c>
-      <c r="AC5" s="5">
-        <v>1</v>
       </c>
       <c r="AD5" s="5">
         <v>77</v>
@@ -1728,10 +1621,10 @@
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>240</v>
+        <v>184</v>
       </c>
       <c r="B6" s="5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -1740,7 +1633,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="5">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
@@ -1752,25 +1645,25 @@
         <v>0</v>
       </c>
       <c r="I6" s="5">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="J6" s="5">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K6" s="5">
         <v>0</v>
       </c>
       <c r="L6" s="5">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="M6" s="5">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="N6" s="5">
         <v>0</v>
       </c>
       <c r="O6" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P6" s="5">
         <v>128</v>
@@ -1809,10 +1702,10 @@
         <v>0</v>
       </c>
       <c r="AB6" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD6" s="5">
         <v>77</v>
@@ -1874,53 +1767,53 @@
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>207</v>
+        <v>240</v>
       </c>
       <c r="B7" s="5">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C7" s="5">
         <v>0</v>
       </c>
       <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>108</v>
+      </c>
+      <c r="J7" s="5">
+        <v>17</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>6</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>3</v>
+      </c>
+      <c r="P7" s="5">
         <v>128</v>
       </c>
-      <c r="E7" s="5">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>38</v>
-      </c>
-      <c r="J7" s="5">
-        <v>6</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>128</v>
-      </c>
-      <c r="M7" s="5">
-        <v>24</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <v>4</v>
-      </c>
-      <c r="P7" s="5">
-        <v>0</v>
-      </c>
       <c r="Q7" s="5">
         <v>0</v>
       </c>
@@ -1949,16 +1842,16 @@
         <v>0</v>
       </c>
       <c r="Z7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>3</v>
+      </c>
+      <c r="AC7" s="5">
         <v>2</v>
-      </c>
-      <c r="AA7" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="5">
-        <v>4</v>
-      </c>
-      <c r="AC7" s="5">
-        <v>1</v>
       </c>
       <c r="AD7" s="5">
         <v>77</v>
@@ -2018,297 +1911,414 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A17" s="5">
-        <v>0</v>
-      </c>
-      <c r="B17" s="5">
-        <v>0</v>
-      </c>
-      <c r="C17" s="5">
-        <v>0</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>207</v>
+      </c>
+      <c r="B8" s="5">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <v>128</v>
+      </c>
+      <c r="E8" s="5">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>38</v>
+      </c>
+      <c r="J8" s="5">
+        <v>6</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="5">
+        <v>128</v>
+      </c>
+      <c r="M8" s="5">
+        <v>24</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
+        <v>4</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0</v>
+      </c>
+      <c r="T8" s="5">
+        <v>0</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+      <c r="V8" s="5">
+        <v>0</v>
+      </c>
+      <c r="W8" s="5">
+        <v>0</v>
+      </c>
+      <c r="X8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>77</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>128</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>255</v>
+      </c>
+      <c r="AM8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" s="8" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="W14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="X14" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f>A3</f>
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:AV15" si="0">B3</f>
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="J17" s="5">
-        <v>1</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="5">
-        <v>26</v>
-      </c>
-      <c r="P17" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="5">
-        <v>0</v>
-      </c>
-      <c r="R17" s="5">
-        <v>0</v>
-      </c>
-      <c r="S17" s="5">
-        <v>0</v>
-      </c>
-      <c r="T17" s="5">
-        <v>0</v>
-      </c>
-      <c r="U17" s="5">
-        <v>0</v>
-      </c>
-      <c r="V17" s="5">
-        <v>0</v>
-      </c>
-      <c r="W17" s="5">
-        <v>0</v>
-      </c>
-      <c r="X17" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="5">
-        <v>188</v>
-      </c>
-      <c r="Z17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD17" s="5">
-        <v>77</v>
-      </c>
-      <c r="AE17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF17" s="5">
-        <v>128</v>
-      </c>
-      <c r="AG17" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AM17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AO17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU17" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV17" s="5">
-        <v>0</v>
+      <c r="AB15">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="AC15">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="AD15">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="AF15">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="AJ15">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="AK15">
+        <f>AK3</f>
+        <v>36</v>
+      </c>
+      <c r="AL15">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="AR15">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="AS15">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="AT15">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="AU15">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="AV15">
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
-        <v>0</v>
-      </c>
-      <c r="B18" s="5">
-        <v>0</v>
-      </c>
-      <c r="C18" s="5">
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <v>26</v>
-      </c>
-      <c r="J18" s="5">
-        <v>1</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-      <c r="M18" s="5">
-        <v>0</v>
-      </c>
-      <c r="N18" s="5">
-        <v>0</v>
-      </c>
-      <c r="O18" s="5">
-        <v>26</v>
-      </c>
-      <c r="P18" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="5">
-        <v>0</v>
-      </c>
-      <c r="R18" s="5">
-        <v>0</v>
-      </c>
-      <c r="S18" s="5">
-        <v>0</v>
-      </c>
-      <c r="T18" s="5">
-        <v>0</v>
-      </c>
-      <c r="U18" s="5">
-        <v>0</v>
-      </c>
-      <c r="V18" s="5">
-        <v>0</v>
-      </c>
-      <c r="W18" s="5">
-        <v>0</v>
-      </c>
-      <c r="X18" s="5">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="5">
-        <v>188</v>
-      </c>
-      <c r="Z18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="5">
-        <v>2</v>
-      </c>
-      <c r="AD18" s="5">
-        <v>77</v>
-      </c>
-      <c r="AE18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AF18" s="5">
-        <v>128</v>
-      </c>
-      <c r="AG18" s="5">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AI18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AK18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AL18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AM18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AN18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AO18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AP18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AQ18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AR18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AS18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AT18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AU18" s="5">
-        <v>0</v>
-      </c>
-      <c r="AV18" s="5">
-        <v>0</v>
-      </c>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="5"/>
+      <c r="AB18" s="5"/>
+      <c r="AC18" s="5"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
+      <c r="AH18" s="5"/>
+      <c r="AI18" s="5"/>
+      <c r="AJ18" s="5"/>
+      <c r="AK18" s="5"/>
+      <c r="AL18" s="5"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+      <c r="AP18" s="5"/>
+      <c r="AQ18" s="5"/>
+      <c r="AR18" s="5"/>
+      <c r="AS18" s="5"/>
+      <c r="AT18" s="5"/>
+      <c r="AU18" s="5"/>
+      <c r="AV18" s="5"/>
     </row>
     <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
@@ -2411,150 +2421,54 @@
       <c r="AV20" s="5"/>
     </row>
     <row r="21" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>26</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>26</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>0</v>
-      </c>
-      <c r="R21">
-        <v>0</v>
-      </c>
-      <c r="S21">
-        <v>0</v>
-      </c>
-      <c r="T21">
-        <v>0</v>
-      </c>
-      <c r="U21">
-        <v>0</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="W21">
-        <v>0</v>
-      </c>
-      <c r="X21">
-        <v>0</v>
-      </c>
-      <c r="Y21">
-        <v>188</v>
-      </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21">
-        <v>0</v>
-      </c>
-      <c r="AB21">
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <v>2</v>
-      </c>
-      <c r="AD21">
-        <v>77</v>
-      </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
-      <c r="AF21">
-        <v>128</v>
-      </c>
-      <c r="AG21">
-        <v>1</v>
-      </c>
-      <c r="AH21">
-        <v>0</v>
-      </c>
-      <c r="AI21">
-        <v>0</v>
-      </c>
-      <c r="AJ21">
-        <v>0</v>
-      </c>
-      <c r="AK21">
-        <v>0</v>
-      </c>
-      <c r="AL21">
-        <v>0</v>
-      </c>
-      <c r="AM21">
-        <v>0</v>
-      </c>
-      <c r="AN21">
-        <v>0</v>
-      </c>
-      <c r="AO21">
-        <v>0</v>
-      </c>
-      <c r="AP21">
-        <v>0</v>
-      </c>
-      <c r="AQ21">
-        <v>0</v>
-      </c>
-      <c r="AR21">
-        <v>0</v>
-      </c>
-      <c r="AS21">
-        <v>0</v>
-      </c>
-      <c r="AT21">
-        <v>0</v>
-      </c>
-      <c r="AU21">
-        <v>0</v>
-      </c>
-      <c r="AV21">
-        <v>0</v>
-      </c>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="5"/>
+      <c r="AQ21" s="5"/>
+      <c r="AR21" s="5"/>
+      <c r="AS21" s="5"/>
+      <c r="AT21" s="5"/>
+      <c r="AU21" s="5"/>
+      <c r="AV21" s="5"/>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -2702,149 +2616,295 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>26</v>
       </c>
-      <c r="J26">
+      <c r="J23">
         <v>1</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
         <v>26</v>
       </c>
-      <c r="P26">
+      <c r="P23">
         <v>1</v>
       </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-      <c r="V26">
-        <v>0</v>
-      </c>
-      <c r="W26">
-        <v>0</v>
-      </c>
-      <c r="X26">
-        <v>0</v>
-      </c>
-      <c r="Y26">
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
         <v>188</v>
       </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AA26">
-        <v>0</v>
-      </c>
-      <c r="AB26">
-        <v>0</v>
-      </c>
-      <c r="AC26">
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
         <v>2</v>
       </c>
-      <c r="AD26">
+      <c r="AD23">
         <v>77</v>
       </c>
-      <c r="AE26">
-        <v>0</v>
-      </c>
-      <c r="AF26">
+      <c r="AE23">
+        <v>0</v>
+      </c>
+      <c r="AF23">
         <v>128</v>
       </c>
-      <c r="AG26">
+      <c r="AG23">
         <v>1</v>
       </c>
-      <c r="AH26">
-        <v>0</v>
-      </c>
-      <c r="AI26">
-        <v>0</v>
-      </c>
-      <c r="AJ26">
-        <v>0</v>
-      </c>
-      <c r="AK26">
-        <v>0</v>
-      </c>
-      <c r="AL26">
-        <v>0</v>
-      </c>
-      <c r="AM26">
-        <v>0</v>
-      </c>
-      <c r="AN26">
-        <v>0</v>
-      </c>
-      <c r="AO26">
-        <v>0</v>
-      </c>
-      <c r="AP26">
-        <v>0</v>
-      </c>
-      <c r="AQ26">
-        <v>0</v>
-      </c>
-      <c r="AR26">
-        <v>0</v>
-      </c>
-      <c r="AS26">
-        <v>0</v>
-      </c>
-      <c r="AT26">
-        <v>0</v>
-      </c>
-      <c r="AU26">
-        <v>0</v>
-      </c>
-      <c r="AV26">
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>0</v>
+      </c>
+      <c r="AL23">
+        <v>0</v>
+      </c>
+      <c r="AM23">
+        <v>0</v>
+      </c>
+      <c r="AN23">
+        <v>0</v>
+      </c>
+      <c r="AO23">
+        <v>0</v>
+      </c>
+      <c r="AP23">
+        <v>0</v>
+      </c>
+      <c r="AQ23">
+        <v>0</v>
+      </c>
+      <c r="AR23">
+        <v>0</v>
+      </c>
+      <c r="AS23">
+        <v>0</v>
+      </c>
+      <c r="AT23">
+        <v>0</v>
+      </c>
+      <c r="AU23">
+        <v>0</v>
+      </c>
+      <c r="AV23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>26</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>188</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>2</v>
+      </c>
+      <c r="AD27">
+        <v>77</v>
+      </c>
+      <c r="AE27">
+        <v>0</v>
+      </c>
+      <c r="AF27">
+        <v>128</v>
+      </c>
+      <c r="AG27">
+        <v>1</v>
+      </c>
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>0</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+      <c r="AM27">
+        <v>0</v>
+      </c>
+      <c r="AN27">
+        <v>0</v>
+      </c>
+      <c r="AO27">
+        <v>0</v>
+      </c>
+      <c r="AP27">
+        <v>0</v>
+      </c>
+      <c r="AQ27">
+        <v>0</v>
+      </c>
+      <c r="AR27">
+        <v>0</v>
+      </c>
+      <c r="AS27">
+        <v>0</v>
+      </c>
+      <c r="AT27">
+        <v>0</v>
+      </c>
+      <c r="AU27">
+        <v>0</v>
+      </c>
+      <c r="AV27">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
func wegArrayMitWegZ(wegz:Double) ->[UInt8] neu: Drillweg
pfeiltag 22, 24 neu: Drill up/down
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445299D2-E544-A64C-8896-957380107146}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD7871E-8992-A544-8AF3-3CD0DA7D68C9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12220" yWindow="24480" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="12220" yWindow="31680" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1081,7 +1081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C059D-FBB1-A24A-890C-2DC09AAA9BCC}">
   <dimension ref="A1:AV27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
override func report_PWM_Slider(_ sender: NSSlider) neu: PWM Drill
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A081E634-65DE-C642-B163-EAE544393468}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137ACA3B-BB96-B544-8921-CB9CA5745FAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12220" yWindow="24460" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t>schrittexA</t>
   </si>
@@ -166,14 +166,20 @@
     <t>cncstatus</t>
   </si>
   <si>
-    <t>ladeposition</t>
+    <t>ladeposition L</t>
+  </si>
+  <si>
+    <t>ladeposition H</t>
+  </si>
+  <si>
+    <t>sendstatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -215,6 +221,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -236,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -265,6 +278,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1091,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C059D-FBB1-A24A-890C-2DC09AAA9BCC}">
-  <dimension ref="A1:AV27"/>
+  <dimension ref="A1:AV37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="K2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2073,1008 +2089,2381 @@
       </c>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>194</v>
-      </c>
-      <c r="R10" s="2">
+      <c r="A10" s="11">
+        <v>202</v>
+      </c>
+      <c r="B10" s="11">
+        <v>10</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0</v>
+      </c>
+      <c r="D10" s="11">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11">
+        <v>162</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <v>210</v>
+      </c>
+      <c r="J10" s="11">
+        <v>28</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0</v>
+      </c>
+      <c r="L10" s="11">
+        <v>128</v>
+      </c>
+      <c r="M10" s="11">
+        <v>61</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="11">
         <v>2</v>
       </c>
-      <c r="S10" s="2">
-        <v>0</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0</v>
-      </c>
-      <c r="U10" s="2">
+      <c r="P10" s="11">
+        <v>128</v>
+      </c>
+      <c r="Q10" s="11">
+        <v>0</v>
+      </c>
+      <c r="R10" s="11">
+        <v>0</v>
+      </c>
+      <c r="S10" s="11">
+        <v>0</v>
+      </c>
+      <c r="T10" s="11">
+        <v>0</v>
+      </c>
+      <c r="U10" s="11">
+        <v>0</v>
+      </c>
+      <c r="V10" s="11">
+        <v>0</v>
+      </c>
+      <c r="W10" s="11">
+        <v>0</v>
+      </c>
+      <c r="X10" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE10" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF10" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG10" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>132</v>
+      </c>
+      <c r="B11" s="11">
+        <v>15</v>
+      </c>
+      <c r="C11" s="11">
+        <v>0</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="11">
+        <v>89</v>
+      </c>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="11">
+        <v>202</v>
+      </c>
+      <c r="J11" s="11">
+        <v>18</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0</v>
+      </c>
+      <c r="M11" s="11">
+        <v>73</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="11">
+        <v>2</v>
+      </c>
+      <c r="P11" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="11">
+        <v>0</v>
+      </c>
+      <c r="R11" s="11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="11">
+        <v>0</v>
+      </c>
+      <c r="T11" s="11">
+        <v>0</v>
+      </c>
+      <c r="U11" s="11">
+        <v>0</v>
+      </c>
+      <c r="V11" s="11">
+        <v>0</v>
+      </c>
+      <c r="W11" s="11">
+        <v>0</v>
+      </c>
+      <c r="X11" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD11" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE11" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF11" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG11" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>113</v>
+      </c>
+      <c r="B12" s="11">
+        <v>17</v>
+      </c>
+      <c r="C12" s="11">
+        <v>0</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+      <c r="E12" s="11">
+        <v>70</v>
+      </c>
+      <c r="F12" s="11">
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0</v>
+      </c>
+      <c r="I12" s="11">
+        <v>132</v>
+      </c>
+      <c r="J12" s="11">
+        <v>12</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0</v>
+      </c>
+      <c r="L12" s="11">
+        <v>128</v>
+      </c>
+      <c r="M12" s="11">
+        <v>98</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0</v>
+      </c>
+      <c r="O12" s="11">
+        <v>2</v>
+      </c>
+      <c r="P12" s="11">
+        <v>128</v>
+      </c>
+      <c r="Q12" s="11">
+        <v>0</v>
+      </c>
+      <c r="R12" s="11">
+        <v>0</v>
+      </c>
+      <c r="S12" s="11">
+        <v>0</v>
+      </c>
+      <c r="T12" s="11">
+        <v>0</v>
+      </c>
+      <c r="U12" s="11">
+        <v>0</v>
+      </c>
+      <c r="V12" s="11">
+        <v>0</v>
+      </c>
+      <c r="W12" s="11">
+        <v>0</v>
+      </c>
+      <c r="X12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="11">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE12" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF12" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG12" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>223</v>
+      </c>
+      <c r="B13" s="11">
+        <v>5</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <v>85</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>216</v>
+      </c>
+      <c r="J13" s="11">
+        <v>34</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0</v>
+      </c>
+      <c r="M13" s="11">
         <v>57</v>
       </c>
-      <c r="V10" s="2">
-        <v>0</v>
-      </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-      <c r="X10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="2">
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
+      <c r="O13" s="11">
+        <v>2</v>
+      </c>
+      <c r="P13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="11">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
+        <v>0</v>
+      </c>
+      <c r="S13" s="11">
+        <v>0</v>
+      </c>
+      <c r="T13" s="11">
+        <v>0</v>
+      </c>
+      <c r="U13" s="11">
+        <v>0</v>
+      </c>
+      <c r="V13" s="11">
+        <v>0</v>
+      </c>
+      <c r="W13" s="11">
+        <v>0</v>
+      </c>
+      <c r="X13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="11">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD13" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE13" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF13" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>159</v>
+      </c>
+      <c r="B14" s="11">
+        <v>49</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>128</v>
+      </c>
+      <c r="E14" s="11">
+        <v>58</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0</v>
+      </c>
+      <c r="I14" s="11">
+        <v>77</v>
+      </c>
+      <c r="J14" s="11">
+        <v>12</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0</v>
+      </c>
+      <c r="L14" s="11">
+        <v>128</v>
+      </c>
+      <c r="M14" s="11">
+        <v>234</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="11">
+        <v>34</v>
+      </c>
+      <c r="P14" s="11">
+        <v>128</v>
+      </c>
+      <c r="Q14" s="11">
+        <v>0</v>
+      </c>
+      <c r="R14" s="11">
+        <v>0</v>
+      </c>
+      <c r="S14" s="11">
+        <v>0</v>
+      </c>
+      <c r="T14" s="11">
+        <v>0</v>
+      </c>
+      <c r="U14" s="11">
+        <v>0</v>
+      </c>
+      <c r="V14" s="11">
+        <v>0</v>
+      </c>
+      <c r="W14" s="11">
+        <v>0</v>
+      </c>
+      <c r="X14" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="11">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="11">
         <v>4</v>
       </c>
-      <c r="AD10" s="2">
+      <c r="AC14" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="11">
         <v>77</v>
       </c>
-      <c r="AE10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="2">
+      <c r="AE14" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF14" s="11">
         <v>128</v>
       </c>
-      <c r="AG10" s="2">
+      <c r="AG14" s="11">
         <v>1</v>
       </c>
-      <c r="AH10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="AH14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="11"/>
+      <c r="Z15" s="11"/>
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="11"/>
+      <c r="AC15" s="11"/>
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="11"/>
+      <c r="AF15" s="11"/>
+      <c r="AG15" s="11"/>
+      <c r="AH15" s="11"/>
+      <c r="AI15" s="11"/>
+      <c r="AJ15" s="11"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="11"/>
+      <c r="AM15" s="11"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="11"/>
+      <c r="AP15" s="11"/>
+      <c r="AQ15" s="11"/>
+      <c r="AR15" s="11"/>
+      <c r="AS15" s="11"/>
+      <c r="AT15" s="11"/>
+      <c r="AU15" s="11"/>
+      <c r="AV15" s="11"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>94</v>
+      </c>
+      <c r="B16" s="11">
+        <v>26</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0</v>
+      </c>
+      <c r="E16" s="11">
+        <v>74</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0</v>
+      </c>
+      <c r="H16" s="11">
+        <v>0</v>
+      </c>
+      <c r="I16" s="11">
+        <v>111</v>
+      </c>
+      <c r="J16" s="11">
+        <v>22</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="11">
+        <v>88</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0</v>
+      </c>
+      <c r="O16" s="11">
+        <v>3</v>
+      </c>
+      <c r="P16" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="11">
+        <v>0</v>
+      </c>
+      <c r="R16" s="11">
+        <v>0</v>
+      </c>
+      <c r="S16" s="11">
+        <v>0</v>
+      </c>
+      <c r="T16" s="11">
+        <v>0</v>
+      </c>
+      <c r="U16" s="11">
+        <v>0</v>
+      </c>
+      <c r="V16" s="11">
+        <v>0</v>
+      </c>
+      <c r="W16" s="11">
+        <v>0</v>
+      </c>
+      <c r="X16" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD16" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE16" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF16" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG16" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>0</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+      <c r="E17" s="11">
+        <v>0</v>
+      </c>
+      <c r="F17" s="11">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11">
+        <v>0</v>
+      </c>
+      <c r="H17" s="11">
+        <v>0</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0</v>
+      </c>
+      <c r="K17" s="11">
+        <v>0</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+      <c r="O17" s="11">
+        <v>0</v>
+      </c>
+      <c r="P17" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>131</v>
+      </c>
+      <c r="R17" s="11">
+        <v>5</v>
+      </c>
+      <c r="S17" s="11">
+        <v>0</v>
+      </c>
+      <c r="T17" s="11">
+        <v>0</v>
+      </c>
+      <c r="U17" s="11">
+        <v>0</v>
+      </c>
+      <c r="V17" s="11">
+        <v>0</v>
+      </c>
+      <c r="W17" s="11">
+        <v>0</v>
+      </c>
+      <c r="X17" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="11">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="11">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG17" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>133</v>
+      </c>
+      <c r="B18" s="11">
+        <v>17</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0</v>
+      </c>
+      <c r="E18" s="11">
+        <v>123</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="11">
+        <v>187</v>
+      </c>
+      <c r="J18" s="11">
+        <v>33</v>
+      </c>
+      <c r="K18" s="11">
+        <v>0</v>
+      </c>
+      <c r="L18" s="11">
+        <v>128</v>
+      </c>
+      <c r="M18" s="11">
+        <v>64</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0</v>
+      </c>
+      <c r="O18" s="11">
+        <v>8</v>
+      </c>
+      <c r="P18" s="11">
+        <v>128</v>
+      </c>
+      <c r="Q18" s="11">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
+        <v>0</v>
+      </c>
+      <c r="S18" s="11">
+        <v>0</v>
+      </c>
+      <c r="T18" s="11">
+        <v>0</v>
+      </c>
+      <c r="U18" s="11">
+        <v>0</v>
+      </c>
+      <c r="V18" s="11">
+        <v>0</v>
+      </c>
+      <c r="W18" s="11">
+        <v>0</v>
+      </c>
+      <c r="X18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="11">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="11">
+        <v>2</v>
+      </c>
+      <c r="AD18" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE18" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF18" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG18" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU18" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>0</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0</v>
+      </c>
+      <c r="F19" s="11">
+        <v>0</v>
+      </c>
+      <c r="G19" s="11">
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
+        <v>0</v>
+      </c>
+      <c r="I19" s="11">
+        <v>0</v>
+      </c>
+      <c r="J19" s="11">
+        <v>0</v>
+      </c>
+      <c r="K19" s="11">
+        <v>0</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0</v>
+      </c>
+      <c r="M19" s="11">
+        <v>0</v>
+      </c>
+      <c r="N19" s="11">
+        <v>0</v>
+      </c>
+      <c r="O19" s="11">
+        <v>0</v>
+      </c>
+      <c r="P19" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="11">
+        <v>131</v>
+      </c>
+      <c r="R19" s="11">
+        <v>5</v>
+      </c>
+      <c r="S19" s="11">
+        <v>0</v>
+      </c>
+      <c r="T19" s="11">
+        <v>0</v>
+      </c>
+      <c r="U19" s="11">
+        <v>0</v>
+      </c>
+      <c r="V19" s="11">
+        <v>0</v>
+      </c>
+      <c r="W19" s="11">
+        <v>0</v>
+      </c>
+      <c r="X19" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="11">
+        <v>3</v>
+      </c>
+      <c r="AC19" s="11">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AF19" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG19" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AM19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU19" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>71</v>
+      </c>
+      <c r="B20" s="11">
+        <v>44</v>
+      </c>
+      <c r="C20" s="11">
+        <v>0</v>
+      </c>
+      <c r="D20" s="11">
+        <v>128</v>
+      </c>
+      <c r="E20" s="11">
+        <v>59</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <v>0</v>
+      </c>
+      <c r="I20" s="11">
+        <v>76</v>
+      </c>
+      <c r="J20" s="11">
+        <v>11</v>
+      </c>
+      <c r="K20" s="11">
+        <v>0</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0</v>
+      </c>
+      <c r="M20" s="11">
+        <v>231</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0</v>
+      </c>
+      <c r="O20" s="11">
+        <v>4</v>
+      </c>
+      <c r="P20" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="11">
+        <v>0</v>
+      </c>
+      <c r="R20" s="11">
+        <v>0</v>
+      </c>
+      <c r="S20" s="11">
+        <v>0</v>
+      </c>
+      <c r="T20" s="11">
+        <v>0</v>
+      </c>
+      <c r="U20" s="11">
+        <v>0</v>
+      </c>
+      <c r="V20" s="11">
+        <v>0</v>
+      </c>
+      <c r="W20" s="11">
+        <v>0</v>
+      </c>
+      <c r="X20" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="11">
+        <v>2</v>
+      </c>
+      <c r="AA20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="11">
+        <v>4</v>
+      </c>
+      <c r="AC20" s="11">
+        <v>1</v>
+      </c>
+      <c r="AD20" s="11">
+        <v>77</v>
+      </c>
+      <c r="AE20" s="11">
+        <v>10</v>
+      </c>
+      <c r="AF20" s="11">
+        <v>128</v>
+      </c>
+      <c r="AG20" s="11">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="11">
+        <v>255</v>
+      </c>
+      <c r="AM20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:48" s="6" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F14" s="6" t="s">
+    <row r="24" spans="1:48" s="6" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="H24" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="T14" s="6" t="s">
+      <c r="J24" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="U14" s="6" t="s">
+      <c r="U24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="W14" s="6" t="s">
+      <c r="W24" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="X14" s="7" t="s">
+      <c r="X24" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A25">
         <f>A3</f>
         <v>0</v>
       </c>
-      <c r="B15">
-        <f t="shared" ref="B15:AV15" si="0">B3</f>
+      <c r="B25">
+        <f t="shared" ref="B25:AV25" si="0">B3</f>
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E15">
+      <c r="E25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F15">
+      <c r="F25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G15">
+      <c r="G25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H15">
+      <c r="H25">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I15">
+      <c r="I25">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J15">
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="K15">
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="L15">
+      <c r="L25">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="M15">
+      <c r="M25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="N15">
+      <c r="N25">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="O15">
+      <c r="O25">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="P15">
+      <c r="P25">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="Q15">
+      <c r="Q25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="R15">
+      <c r="R25">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="S15">
+      <c r="S25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="T15">
+      <c r="T25">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="U15">
+      <c r="U25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="V15">
+      <c r="V25">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="W15">
+      <c r="W25">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="X15">
+      <c r="X25">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="Y15">
+      <c r="Y25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="Z15">
+      <c r="Z25">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AA15">
+      <c r="AA25">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AB15">
+      <c r="AB25">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AC15">
+      <c r="AC25">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AD15">
+      <c r="AD25">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AE15">
+      <c r="AE25">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AF15">
+      <c r="AF25">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AG15">
+      <c r="AG25">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AH15">
+      <c r="AH25">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AI15">
+      <c r="AI25">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AJ15">
+      <c r="AJ25">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AK15">
+      <c r="AK25">
         <f>AK3</f>
         <v>36</v>
       </c>
-      <c r="AL15">
+      <c r="AL25">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AM15">
+      <c r="AM25">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AN15">
+      <c r="AN25">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AO15">
+      <c r="AO25">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AP15">
+      <c r="AP25">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AQ15">
+      <c r="AQ25">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AR15">
+      <c r="AR25">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AS15">
+      <c r="AS25">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AT15">
+      <c r="AT25">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AU15">
+      <c r="AU25">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AV15">
+      <c r="AV25">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="5"/>
-      <c r="W18" s="5"/>
-      <c r="X18" s="5"/>
-      <c r="Y18" s="5"/>
-      <c r="Z18" s="5"/>
-      <c r="AA18" s="5"/>
-      <c r="AB18" s="5"/>
-      <c r="AC18" s="5"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="5"/>
-      <c r="AF18" s="5"/>
-      <c r="AG18" s="5"/>
-      <c r="AH18" s="5"/>
-      <c r="AI18" s="5"/>
-      <c r="AJ18" s="5"/>
-      <c r="AK18" s="5"/>
-      <c r="AL18" s="5"/>
-      <c r="AM18" s="5"/>
-      <c r="AN18" s="5"/>
-      <c r="AO18" s="5"/>
-      <c r="AP18" s="5"/>
-      <c r="AQ18" s="5"/>
-      <c r="AR18" s="5"/>
-      <c r="AS18" s="5"/>
-      <c r="AT18" s="5"/>
-      <c r="AU18" s="5"/>
-      <c r="AV18" s="5"/>
-    </row>
-    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="5"/>
-      <c r="AG19" s="5"/>
-      <c r="AH19" s="5"/>
-      <c r="AI19" s="5"/>
-      <c r="AJ19" s="5"/>
-      <c r="AK19" s="5"/>
-      <c r="AL19" s="5"/>
-      <c r="AM19" s="5"/>
-      <c r="AN19" s="5"/>
-      <c r="AO19" s="5"/>
-      <c r="AP19" s="5"/>
-      <c r="AQ19" s="5"/>
-      <c r="AR19" s="5"/>
-      <c r="AS19" s="5"/>
-      <c r="AT19" s="5"/>
-      <c r="AU19" s="5"/>
-      <c r="AV19" s="5"/>
-    </row>
-    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-      <c r="Z20" s="5"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="5"/>
-      <c r="AC20" s="5"/>
-      <c r="AD20" s="5"/>
-      <c r="AE20" s="5"/>
-      <c r="AF20" s="5"/>
-      <c r="AG20" s="5"/>
-      <c r="AH20" s="5"/>
-      <c r="AI20" s="5"/>
-      <c r="AJ20" s="5"/>
-      <c r="AK20" s="5"/>
-      <c r="AL20" s="5"/>
-      <c r="AM20" s="5"/>
-      <c r="AN20" s="5"/>
-      <c r="AO20" s="5"/>
-      <c r="AP20" s="5"/>
-      <c r="AQ20" s="5"/>
-      <c r="AR20" s="5"/>
-      <c r="AS20" s="5"/>
-      <c r="AT20" s="5"/>
-      <c r="AU20" s="5"/>
-      <c r="AV20" s="5"/>
-    </row>
-    <row r="21" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="5"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="5"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="5"/>
-      <c r="AG21" s="5"/>
-      <c r="AH21" s="5"/>
-      <c r="AI21" s="5"/>
-      <c r="AJ21" s="5"/>
-      <c r="AK21" s="5"/>
-      <c r="AL21" s="5"/>
-      <c r="AM21" s="5"/>
-      <c r="AN21" s="5"/>
-      <c r="AO21" s="5"/>
-      <c r="AP21" s="5"/>
-      <c r="AQ21" s="5"/>
-      <c r="AR21" s="5"/>
-      <c r="AS21" s="5"/>
-      <c r="AT21" s="5"/>
-      <c r="AU21" s="5"/>
-      <c r="AV21" s="5"/>
-    </row>
-    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
+    <row r="28" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="5"/>
+      <c r="AO28" s="5"/>
+      <c r="AP28" s="5"/>
+      <c r="AQ28" s="5"/>
+      <c r="AR28" s="5"/>
+      <c r="AS28" s="5"/>
+      <c r="AT28" s="5"/>
+      <c r="AU28" s="5"/>
+      <c r="AV28" s="5"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="5"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="5"/>
+      <c r="AO29" s="5"/>
+      <c r="AP29" s="5"/>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="5"/>
+      <c r="AS29" s="5"/>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="5"/>
+      <c r="AV29" s="5"/>
+    </row>
+    <row r="30" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="5"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="5"/>
+      <c r="AO30" s="5"/>
+      <c r="AP30" s="5"/>
+      <c r="AQ30" s="5"/>
+      <c r="AR30" s="5"/>
+      <c r="AS30" s="5"/>
+      <c r="AT30" s="5"/>
+      <c r="AU30" s="5"/>
+      <c r="AV30" s="5"/>
+    </row>
+    <row r="31" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="5"/>
+      <c r="AO31" s="5"/>
+      <c r="AP31" s="5"/>
+      <c r="AQ31" s="5"/>
+      <c r="AR31" s="5"/>
+      <c r="AS31" s="5"/>
+      <c r="AT31" s="5"/>
+      <c r="AU31" s="5"/>
+      <c r="AV31" s="5"/>
+    </row>
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
         <v>26</v>
       </c>
-      <c r="J22">
+      <c r="J32">
         <v>1</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
         <v>26</v>
       </c>
-      <c r="P22">
+      <c r="P32">
         <v>1</v>
       </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>0</v>
-      </c>
-      <c r="U22">
-        <v>0</v>
-      </c>
-      <c r="V22">
-        <v>0</v>
-      </c>
-      <c r="W22">
-        <v>0</v>
-      </c>
-      <c r="X22">
-        <v>0</v>
-      </c>
-      <c r="Y22">
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
         <v>188</v>
       </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AA22">
-        <v>0</v>
-      </c>
-      <c r="AB22">
-        <v>0</v>
-      </c>
-      <c r="AC22">
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>0</v>
+      </c>
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32">
         <v>2</v>
       </c>
-      <c r="AD22">
+      <c r="AD32">
         <v>77</v>
       </c>
-      <c r="AE22">
-        <v>0</v>
-      </c>
-      <c r="AF22">
+      <c r="AE32">
+        <v>0</v>
+      </c>
+      <c r="AF32">
         <v>128</v>
       </c>
-      <c r="AG22">
+      <c r="AG32">
         <v>1</v>
       </c>
-      <c r="AH22">
-        <v>0</v>
-      </c>
-      <c r="AI22">
-        <v>0</v>
-      </c>
-      <c r="AJ22">
-        <v>0</v>
-      </c>
-      <c r="AK22">
-        <v>0</v>
-      </c>
-      <c r="AL22">
-        <v>0</v>
-      </c>
-      <c r="AM22">
-        <v>0</v>
-      </c>
-      <c r="AN22">
-        <v>0</v>
-      </c>
-      <c r="AO22">
-        <v>0</v>
-      </c>
-      <c r="AP22">
-        <v>0</v>
-      </c>
-      <c r="AQ22">
-        <v>0</v>
-      </c>
-      <c r="AR22">
-        <v>0</v>
-      </c>
-      <c r="AS22">
-        <v>0</v>
-      </c>
-      <c r="AT22">
-        <v>0</v>
-      </c>
-      <c r="AU22">
-        <v>0</v>
-      </c>
-      <c r="AV22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
+      <c r="AH32">
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>0</v>
+      </c>
+      <c r="AM32">
+        <v>0</v>
+      </c>
+      <c r="AN32">
+        <v>0</v>
+      </c>
+      <c r="AO32">
+        <v>0</v>
+      </c>
+      <c r="AP32">
+        <v>0</v>
+      </c>
+      <c r="AQ32">
+        <v>0</v>
+      </c>
+      <c r="AR32">
+        <v>0</v>
+      </c>
+      <c r="AS32">
+        <v>0</v>
+      </c>
+      <c r="AT32">
+        <v>0</v>
+      </c>
+      <c r="AU32">
+        <v>0</v>
+      </c>
+      <c r="AV32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
         <v>26</v>
       </c>
-      <c r="J23">
+      <c r="J33">
         <v>1</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
         <v>26</v>
       </c>
-      <c r="P23">
+      <c r="P33">
         <v>1</v>
       </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>0</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-      <c r="V23">
-        <v>0</v>
-      </c>
-      <c r="W23">
-        <v>0</v>
-      </c>
-      <c r="X23">
-        <v>0</v>
-      </c>
-      <c r="Y23">
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>0</v>
+      </c>
+      <c r="T33">
+        <v>0</v>
+      </c>
+      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
+        <v>0</v>
+      </c>
+      <c r="W33">
+        <v>0</v>
+      </c>
+      <c r="X33">
+        <v>0</v>
+      </c>
+      <c r="Y33">
         <v>188</v>
       </c>
-      <c r="Z23">
-        <v>0</v>
-      </c>
-      <c r="AA23">
-        <v>0</v>
-      </c>
-      <c r="AB23">
-        <v>0</v>
-      </c>
-      <c r="AC23">
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>0</v>
+      </c>
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33">
         <v>2</v>
       </c>
-      <c r="AD23">
+      <c r="AD33">
         <v>77</v>
       </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-      <c r="AF23">
+      <c r="AE33">
+        <v>0</v>
+      </c>
+      <c r="AF33">
         <v>128</v>
       </c>
-      <c r="AG23">
+      <c r="AG33">
         <v>1</v>
       </c>
-      <c r="AH23">
-        <v>0</v>
-      </c>
-      <c r="AI23">
-        <v>0</v>
-      </c>
-      <c r="AJ23">
-        <v>0</v>
-      </c>
-      <c r="AK23">
-        <v>0</v>
-      </c>
-      <c r="AL23">
-        <v>0</v>
-      </c>
-      <c r="AM23">
-        <v>0</v>
-      </c>
-      <c r="AN23">
-        <v>0</v>
-      </c>
-      <c r="AO23">
-        <v>0</v>
-      </c>
-      <c r="AP23">
-        <v>0</v>
-      </c>
-      <c r="AQ23">
-        <v>0</v>
-      </c>
-      <c r="AR23">
-        <v>0</v>
-      </c>
-      <c r="AS23">
-        <v>0</v>
-      </c>
-      <c r="AT23">
-        <v>0</v>
-      </c>
-      <c r="AU23">
-        <v>0</v>
-      </c>
-      <c r="AV23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>0</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+      <c r="AM33">
+        <v>0</v>
+      </c>
+      <c r="AN33">
+        <v>0</v>
+      </c>
+      <c r="AO33">
+        <v>0</v>
+      </c>
+      <c r="AP33">
+        <v>0</v>
+      </c>
+      <c r="AQ33">
+        <v>0</v>
+      </c>
+      <c r="AR33">
+        <v>0</v>
+      </c>
+      <c r="AS33">
+        <v>0</v>
+      </c>
+      <c r="AT33">
+        <v>0</v>
+      </c>
+      <c r="AU33">
+        <v>0</v>
+      </c>
+      <c r="AV33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
         <v>26</v>
       </c>
-      <c r="J27">
+      <c r="J37">
         <v>1</v>
       </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
         <v>26</v>
       </c>
-      <c r="P27">
+      <c r="P37">
         <v>1</v>
       </c>
-      <c r="Q27">
-        <v>0</v>
-      </c>
-      <c r="R27">
-        <v>0</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>0</v>
-      </c>
-      <c r="V27">
-        <v>0</v>
-      </c>
-      <c r="W27">
-        <v>0</v>
-      </c>
-      <c r="X27">
-        <v>0</v>
-      </c>
-      <c r="Y27">
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>0</v>
+      </c>
+      <c r="U37">
+        <v>0</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0</v>
+      </c>
+      <c r="X37">
+        <v>0</v>
+      </c>
+      <c r="Y37">
         <v>188</v>
       </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AA27">
-        <v>0</v>
-      </c>
-      <c r="AB27">
-        <v>0</v>
-      </c>
-      <c r="AC27">
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>0</v>
+      </c>
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37">
         <v>2</v>
       </c>
-      <c r="AD27">
+      <c r="AD37">
         <v>77</v>
       </c>
-      <c r="AE27">
-        <v>0</v>
-      </c>
-      <c r="AF27">
+      <c r="AE37">
+        <v>0</v>
+      </c>
+      <c r="AF37">
         <v>128</v>
       </c>
-      <c r="AG27">
+      <c r="AG37">
         <v>1</v>
       </c>
-      <c r="AH27">
-        <v>0</v>
-      </c>
-      <c r="AI27">
-        <v>0</v>
-      </c>
-      <c r="AJ27">
-        <v>0</v>
-      </c>
-      <c r="AK27">
-        <v>0</v>
-      </c>
-      <c r="AL27">
-        <v>0</v>
-      </c>
-      <c r="AM27">
-        <v>0</v>
-      </c>
-      <c r="AN27">
-        <v>0</v>
-      </c>
-      <c r="AO27">
-        <v>0</v>
-      </c>
-      <c r="AP27">
-        <v>0</v>
-      </c>
-      <c r="AQ27">
-        <v>0</v>
-      </c>
-      <c r="AR27">
-        <v>0</v>
-      </c>
-      <c r="AS27">
-        <v>0</v>
-      </c>
-      <c r="AT27">
-        <v>0</v>
-      </c>
-      <c r="AU27">
-        <v>0</v>
-      </c>
-      <c r="AV27">
+      <c r="AH37">
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <v>0</v>
+      </c>
+      <c r="AK37">
+        <v>0</v>
+      </c>
+      <c r="AL37">
+        <v>0</v>
+      </c>
+      <c r="AM37">
+        <v>0</v>
+      </c>
+      <c r="AN37">
+        <v>0</v>
+      </c>
+      <c r="AO37">
+        <v>0</v>
+      </c>
+      <c r="AP37">
+        <v>0</v>
+      </c>
+      <c r="AQ37">
+        <v>0</v>
+      </c>
+      <c r="AR37">
+        <v>0</v>
+      </c>
+      <c r="AS37">
+        <v>0</v>
+      </c>
+      <c r="AT37">
+        <v>0</v>
+      </c>
+      <c r="AU37">
+        <v>0</v>
+      </c>
+      <c r="AV37">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Platteview draw reduzieren: PCB: l 5065 ff anzeigezeile, drillzeile neu [39] bis [42] - drillzeile ist 0xFFFF - anzeigezeile: nur move-zeilen. -mitgeben, für PlatteView
PlatteView:
nur Markfeld neu zeichnen > *** Reduktion CPU-Last!!! ***
      self.setNeedsDisplay(markfeldarray[stepperposition])
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD477108-4BD0-8748-BCCA-57F07BCEE652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85912BDC-76CC-CC4F-86CC-15265E15F7C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="23580" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="12220" yWindow="30780" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>schrittexA</t>
   </si>
@@ -180,6 +180,18 @@
   <si>
     <t>anzabschnitteL</t>
   </si>
+  <si>
+    <t>anzeigezeile H</t>
+  </si>
+  <si>
+    <t>anzeigezeile L</t>
+  </si>
+  <si>
+    <t>drrillzeile H</t>
+  </si>
+  <si>
+    <t>drillzeile L</t>
+  </si>
 </sst>
 </file>
 
@@ -269,7 +281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -313,6 +325,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40 % - Akzent2" xfId="1" builtinId="35"/>
@@ -1141,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C059D-FBB1-A24A-890C-2DC09AAA9BCC}">
   <dimension ref="A1:CR54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:AV11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,6 +1267,21 @@
       <c r="AM2" s="11" t="s">
         <v>44</v>
       </c>
+      <c r="AN2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR2" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -2132,734 +2160,446 @@
       </c>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>202</v>
-      </c>
-      <c r="B10" s="8">
-        <v>10</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8">
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <v>162</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0</v>
-      </c>
-      <c r="I10" s="8">
-        <v>210</v>
-      </c>
-      <c r="J10" s="8">
-        <v>28</v>
-      </c>
-      <c r="K10" s="8">
-        <v>0</v>
-      </c>
-      <c r="L10" s="8">
+      <c r="A10" s="5">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>206</v>
+      </c>
+      <c r="J10" s="5">
+        <v>137</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>0</v>
+      </c>
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>206</v>
+      </c>
+      <c r="P10" s="5">
+        <v>137</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+      <c r="W10" s="5">
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>222</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>77</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="5">
         <v>128</v>
       </c>
-      <c r="M10" s="8">
-        <v>61</v>
-      </c>
-      <c r="N10" s="8">
-        <v>0</v>
-      </c>
-      <c r="O10" s="8">
+      <c r="AG10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="5">
         <v>2</v>
       </c>
-      <c r="P10" s="8">
+      <c r="AN10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:96" x14ac:dyDescent="0.2">
+      <c r="A11" s="17">
+        <v>206</v>
+      </c>
+      <c r="B11" s="17">
+        <v>137</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>57</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
+        <v>0</v>
+      </c>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>0</v>
+      </c>
+      <c r="R11" s="17">
+        <v>0</v>
+      </c>
+      <c r="S11" s="17">
+        <v>0</v>
+      </c>
+      <c r="T11" s="17">
+        <v>0</v>
+      </c>
+      <c r="U11" s="17">
+        <v>0</v>
+      </c>
+      <c r="V11" s="17">
+        <v>0</v>
+      </c>
+      <c r="W11" s="17">
+        <v>0</v>
+      </c>
+      <c r="X11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="17">
+        <v>222</v>
+      </c>
+      <c r="Z11" s="17">
+        <v>2</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AD11" s="17">
+        <v>77</v>
+      </c>
+      <c r="AE11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="17">
         <v>128</v>
       </c>
-      <c r="Q10" s="8">
-        <v>0</v>
-      </c>
-      <c r="R10" s="8">
-        <v>0</v>
-      </c>
-      <c r="S10" s="8">
-        <v>0</v>
-      </c>
-      <c r="T10" s="8">
-        <v>0</v>
-      </c>
-      <c r="U10" s="8">
-        <v>0</v>
-      </c>
-      <c r="V10" s="8">
-        <v>0</v>
-      </c>
-      <c r="W10" s="8">
-        <v>0</v>
-      </c>
-      <c r="X10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="15">
+      <c r="AG11" s="17">
         <v>1</v>
       </c>
-      <c r="AA10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="8">
-        <v>2</v>
-      </c>
-      <c r="AD10" s="8">
-        <v>77</v>
-      </c>
-      <c r="AE10" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF10" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG10" s="8">
+      <c r="AH11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="17">
         <v>1</v>
       </c>
-      <c r="AH10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU10" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV10" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
-        <v>132</v>
-      </c>
-      <c r="B11" s="8">
-        <v>15</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0</v>
-      </c>
-      <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>89</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8">
-        <v>202</v>
-      </c>
-      <c r="J11" s="8">
-        <v>18</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="8">
-        <v>0</v>
-      </c>
-      <c r="M11" s="8">
-        <v>73</v>
-      </c>
-      <c r="N11" s="8">
-        <v>0</v>
-      </c>
-      <c r="O11" s="8">
-        <v>2</v>
-      </c>
-      <c r="P11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>0</v>
-      </c>
-      <c r="R11" s="8">
-        <v>0</v>
-      </c>
-      <c r="S11" s="8">
-        <v>0</v>
-      </c>
-      <c r="T11" s="8">
-        <v>0</v>
-      </c>
-      <c r="U11" s="8">
-        <v>0</v>
-      </c>
-      <c r="V11" s="8">
-        <v>0</v>
-      </c>
-      <c r="W11" s="8">
-        <v>0</v>
-      </c>
-      <c r="X11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="8">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="8">
-        <v>2</v>
-      </c>
-      <c r="AD11" s="8">
-        <v>77</v>
-      </c>
-      <c r="AE11" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF11" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG11" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU11" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV11" s="8">
+      <c r="AN11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="17">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
-        <v>113</v>
-      </c>
-      <c r="B12" s="8">
-        <v>17</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <v>70</v>
-      </c>
-      <c r="F12" s="8">
-        <v>0</v>
-      </c>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8">
-        <v>132</v>
-      </c>
-      <c r="J12" s="8">
-        <v>12</v>
-      </c>
-      <c r="K12" s="8">
-        <v>0</v>
-      </c>
-      <c r="L12" s="8">
-        <v>128</v>
-      </c>
-      <c r="M12" s="8">
-        <v>98</v>
-      </c>
-      <c r="N12" s="8">
-        <v>0</v>
-      </c>
-      <c r="O12" s="8">
-        <v>2</v>
-      </c>
-      <c r="P12" s="8">
-        <v>128</v>
-      </c>
-      <c r="Q12" s="8">
-        <v>0</v>
-      </c>
-      <c r="R12" s="8">
-        <v>0</v>
-      </c>
-      <c r="S12" s="8">
-        <v>0</v>
-      </c>
-      <c r="T12" s="8">
-        <v>0</v>
-      </c>
-      <c r="U12" s="8">
-        <v>0</v>
-      </c>
-      <c r="V12" s="8">
-        <v>0</v>
-      </c>
-      <c r="W12" s="8">
-        <v>0</v>
-      </c>
-      <c r="X12" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="8">
-        <v>2</v>
-      </c>
-      <c r="AC12" s="8">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="8">
-        <v>77</v>
-      </c>
-      <c r="AE12" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF12" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG12" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL12" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU12" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV12" s="8">
-        <v>0</v>
-      </c>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
+      <c r="AM12" s="8"/>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="8"/>
+      <c r="AQ12" s="8"/>
+      <c r="AR12" s="8"/>
+      <c r="AS12" s="8"/>
+      <c r="AT12" s="8"/>
+      <c r="AU12" s="8"/>
+      <c r="AV12" s="8"/>
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
-        <v>223</v>
-      </c>
-      <c r="B13" s="8">
-        <v>5</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0</v>
-      </c>
-      <c r="D13" s="8">
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
-        <v>85</v>
-      </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8">
-        <v>0</v>
-      </c>
-      <c r="I13" s="8">
-        <v>216</v>
-      </c>
-      <c r="J13" s="8">
-        <v>34</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="8">
-        <v>0</v>
-      </c>
-      <c r="M13" s="8">
-        <v>57</v>
-      </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="O13" s="8">
-        <v>2</v>
-      </c>
-      <c r="P13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>0</v>
-      </c>
-      <c r="R13" s="8">
-        <v>0</v>
-      </c>
-      <c r="S13" s="8">
-        <v>0</v>
-      </c>
-      <c r="T13" s="8">
-        <v>0</v>
-      </c>
-      <c r="U13" s="8">
-        <v>0</v>
-      </c>
-      <c r="V13" s="8">
-        <v>0</v>
-      </c>
-      <c r="W13" s="8">
-        <v>0</v>
-      </c>
-      <c r="X13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="15">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="8">
-        <v>3</v>
-      </c>
-      <c r="AC13" s="8">
-        <v>2</v>
-      </c>
-      <c r="AD13" s="8">
-        <v>77</v>
-      </c>
-      <c r="AE13" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF13" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG13" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV13" s="8">
-        <v>0</v>
-      </c>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="15"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="8"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
+      <c r="AM13" s="8"/>
+      <c r="AN13" s="8"/>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="8"/>
+      <c r="AQ13" s="8"/>
+      <c r="AR13" s="8"/>
+      <c r="AS13" s="8"/>
+      <c r="AT13" s="8"/>
+      <c r="AU13" s="8"/>
+      <c r="AV13" s="8"/>
     </row>
     <row r="14" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
-        <v>159</v>
-      </c>
-      <c r="B14" s="8">
-        <v>49</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0</v>
-      </c>
-      <c r="D14" s="8">
-        <v>128</v>
-      </c>
-      <c r="E14" s="8">
-        <v>58</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8">
-        <v>77</v>
-      </c>
-      <c r="J14" s="8">
-        <v>12</v>
-      </c>
-      <c r="K14" s="8">
-        <v>0</v>
-      </c>
-      <c r="L14" s="8">
-        <v>128</v>
-      </c>
-      <c r="M14" s="8">
-        <v>234</v>
-      </c>
-      <c r="N14" s="8">
-        <v>0</v>
-      </c>
-      <c r="O14" s="8">
-        <v>34</v>
-      </c>
-      <c r="P14" s="8">
-        <v>128</v>
-      </c>
-      <c r="Q14" s="8">
-        <v>0</v>
-      </c>
-      <c r="R14" s="8">
-        <v>0</v>
-      </c>
-      <c r="S14" s="8">
-        <v>0</v>
-      </c>
-      <c r="T14" s="8">
-        <v>0</v>
-      </c>
-      <c r="U14" s="8">
-        <v>0</v>
-      </c>
-      <c r="V14" s="8">
-        <v>0</v>
-      </c>
-      <c r="W14" s="8">
-        <v>0</v>
-      </c>
-      <c r="X14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="15">
-        <v>2</v>
-      </c>
-      <c r="AA14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="8">
-        <v>4</v>
-      </c>
-      <c r="AC14" s="8">
-        <v>1</v>
-      </c>
-      <c r="AD14" s="8">
-        <v>77</v>
-      </c>
-      <c r="AE14" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF14" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG14" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL14" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU14" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV14" s="8">
-        <v>0</v>
-      </c>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="15"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
+      <c r="AN14" s="8"/>
+      <c r="AO14" s="8"/>
+      <c r="AP14" s="8"/>
+      <c r="AQ14" s="8"/>
+      <c r="AR14" s="8"/>
+      <c r="AS14" s="8"/>
+      <c r="AT14" s="8"/>
+      <c r="AU14" s="8"/>
+      <c r="AV14" s="8"/>
     </row>
     <row r="15" spans="1:96" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
@@ -2912,150 +2652,54 @@
       <c r="AV15" s="8"/>
     </row>
     <row r="16" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A16" s="8">
-        <v>0</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0</v>
-      </c>
-      <c r="D16" s="8">
-        <v>0</v>
-      </c>
-      <c r="E16" s="8">
-        <v>0</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8">
-        <v>0</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0</v>
-      </c>
-      <c r="J16" s="8">
-        <v>0</v>
-      </c>
-      <c r="K16" s="8">
-        <v>0</v>
-      </c>
-      <c r="L16" s="8">
-        <v>0</v>
-      </c>
-      <c r="M16" s="8">
-        <v>0</v>
-      </c>
-      <c r="N16" s="8">
-        <v>0</v>
-      </c>
-      <c r="O16" s="8">
-        <v>0</v>
-      </c>
-      <c r="P16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>131</v>
-      </c>
-      <c r="R16" s="8">
-        <v>5</v>
-      </c>
-      <c r="S16" s="8">
-        <v>0</v>
-      </c>
-      <c r="T16" s="8">
-        <v>128</v>
-      </c>
-      <c r="U16" s="8">
-        <v>0</v>
-      </c>
-      <c r="V16" s="8">
-        <v>0</v>
-      </c>
-      <c r="W16" s="8">
-        <v>0</v>
-      </c>
-      <c r="X16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="15">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="8">
-        <v>4</v>
-      </c>
-      <c r="AD16" s="8">
-        <v>128</v>
-      </c>
-      <c r="AE16" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF16" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG16" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL16" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU16" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV16" s="8">
-        <v>0</v>
-      </c>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
+      <c r="AL16" s="8"/>
+      <c r="AM16" s="8"/>
+      <c r="AN16" s="8"/>
+      <c r="AO16" s="8"/>
+      <c r="AP16" s="8"/>
+      <c r="AQ16" s="8"/>
+      <c r="AR16" s="8"/>
+      <c r="AS16" s="8"/>
+      <c r="AT16" s="8"/>
+      <c r="AU16" s="8"/>
+      <c r="AV16" s="8"/>
       <c r="AX16" s="12"/>
       <c r="AY16" s="12"/>
       <c r="AZ16" s="12"/>
@@ -3105,150 +2749,54 @@
       <c r="CR16" s="12"/>
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A17" s="8">
-        <v>0</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0</v>
-      </c>
-      <c r="D17" s="8">
-        <v>0</v>
-      </c>
-      <c r="E17" s="8">
-        <v>0</v>
-      </c>
-      <c r="F17" s="8">
-        <v>0</v>
-      </c>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-      <c r="H17" s="8">
-        <v>0</v>
-      </c>
-      <c r="I17" s="8">
-        <v>0</v>
-      </c>
-      <c r="J17" s="8">
-        <v>0</v>
-      </c>
-      <c r="K17" s="8">
-        <v>0</v>
-      </c>
-      <c r="L17" s="8">
-        <v>0</v>
-      </c>
-      <c r="M17" s="8">
-        <v>0</v>
-      </c>
-      <c r="N17" s="8">
-        <v>0</v>
-      </c>
-      <c r="O17" s="8">
-        <v>0</v>
-      </c>
-      <c r="P17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="8">
-        <v>131</v>
-      </c>
-      <c r="R17" s="8">
-        <v>5</v>
-      </c>
-      <c r="S17" s="8">
-        <v>0</v>
-      </c>
-      <c r="T17" s="8">
-        <v>0</v>
-      </c>
-      <c r="U17" s="8">
-        <v>0</v>
-      </c>
-      <c r="V17" s="8">
-        <v>0</v>
-      </c>
-      <c r="W17" s="8">
-        <v>0</v>
-      </c>
-      <c r="X17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="15">
-        <v>2</v>
-      </c>
-      <c r="AA17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="8">
-        <v>1</v>
-      </c>
-      <c r="AC17" s="8">
-        <v>4</v>
-      </c>
-      <c r="AD17" s="8">
-        <v>64</v>
-      </c>
-      <c r="AE17" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF17" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG17" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL17" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU17" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV17" s="8">
-        <v>0</v>
-      </c>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="15"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
+      <c r="AM17" s="8"/>
+      <c r="AN17" s="8"/>
+      <c r="AO17" s="8"/>
+      <c r="AP17" s="8"/>
+      <c r="AQ17" s="8"/>
+      <c r="AR17" s="8"/>
+      <c r="AS17" s="8"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="8"/>
+      <c r="AV17" s="8"/>
       <c r="AW17" s="8"/>
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
report_Motor_Slider neu, code 0xDA, BIT 28
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAB9388-6DE9-3044-BA55-ED8067924D1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F692A79-A4CB-A843-AAA7-CAEFB817A1EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="6080" windowWidth="25600" windowHeight="12200" activeTab="2" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="10660" yWindow="2920" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
   <si>
     <t>schrittexA</t>
   </si>
@@ -312,13 +312,16 @@
   </si>
   <si>
     <t>drillspeed</t>
+  </si>
+  <si>
+    <t>Motor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -374,6 +377,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -402,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -447,6 +458,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40 % - Akzent2" xfId="1" builtinId="35"/>
@@ -1281,14 +1293,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989FA3DE-5878-0046-AD10-653CF00B61CC}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1454,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C059D-FBB1-A24A-890C-2DC09AAA9BCC}">
   <dimension ref="A1:CR54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:AV6"/>
+    <sheetView topLeftCell="S2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1554,6 +1566,9 @@
       </c>
       <c r="AB2" s="9" t="s">
         <v>27</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>95</v>
       </c>
       <c r="AD2" s="10" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
hid: prod, vendor weg
PCB: drill abs , Nullpunkt neu (niht verwendet)
instance var drillweg neu: aus drillwegFeld

drillMoveArray mit direkter Umrechnung mm zu steps

report_drill_up neu mit funktion drill_up

report_Dicke neu: absenken um Platinendicke

PlatteView: flipder Darstellung neu
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F692A79-A4CB-A843-AAA7-CAEFB817A1EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B1BC63-BB8A-D046-87F5-A49C19307F26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="2920" windowWidth="25600" windowHeight="12200" activeTab="1" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="12560" yWindow="22780" windowWidth="25600" windowHeight="12200" activeTab="2" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="114">
   <si>
     <t>schrittexA</t>
   </si>
@@ -315,13 +315,67 @@
   </si>
   <si>
     <t>Motor</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Drilldaten</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>set nullpunkt C</t>
+  </si>
+  <si>
+    <t>report_send_Daten</t>
+  </si>
+  <si>
+    <t>report_DrillspeedSlider</t>
+  </si>
+  <si>
+    <t>report_Drill_Abs_up down</t>
+  </si>
+  <si>
+    <t>report_move_Drill report_Drill_up drill_up down</t>
+  </si>
+  <si>
+    <t>drilltask</t>
+  </si>
+  <si>
+    <t>Meldung start B6</t>
+  </si>
+  <si>
+    <t>Meldung Drill zurueck</t>
+  </si>
+  <si>
+    <t>datatabletask</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>Antwort tabledataaktion</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Anschlag</t>
+  </si>
+  <si>
+    <t>move, report_home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -385,6 +439,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0F68A0"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF267507"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC41A16"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -413,7 +485,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -459,6 +531,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="40 % - Akzent2" xfId="1" builtinId="35"/>
@@ -1291,13 +1372,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{989FA3DE-5878-0046-AD10-653CF00B61CC}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="26.33203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
@@ -1350,10 +1435,21 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>72</v>
       </c>
+      <c r="B12" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="H12" t="s">
         <v>70</v>
       </c>
@@ -1361,15 +1457,43 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="H18" t="s">
         <v>80</v>
       </c>
@@ -1377,83 +1501,142 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" t="s">
+    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>73</v>
       </c>
-      <c r="I20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-      <c r="H22" t="s">
-        <v>77</v>
-      </c>
-      <c r="I22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H23" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" t="s">
-        <v>79</v>
+      <c r="B19" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="19"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="19"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="19"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="19"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="19"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="19"/>
+    </row>
+    <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H40" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" t="s">
+        <v>77</v>
+      </c>
+      <c r="I42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>67</v>
+      </c>
+      <c r="I43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>82</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H45" t="s">
         <v>83</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I45" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>86</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H46" t="s">
         <v>85</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I46" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>90</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H47" t="s">
         <v>87</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="49" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>92</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B49" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H49" t="s">
         <v>91</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I49" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1466,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF1C059D-FBB1-A24A-890C-2DC09AAA9BCC}">
   <dimension ref="A1:CR54"/>
   <sheetViews>
-    <sheetView topLeftCell="S2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
svg-popup-stuff: gewählte Devices speichern
dev_present reduzieren
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B1BC63-BB8A-D046-87F5-A49C19307F26}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4AE1FB-60CB-8B4B-BBED-1340B4894D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12560" yWindow="22780" windowWidth="25600" windowHeight="12200" activeTab="2" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="3100" yWindow="13040" windowWidth="37240" windowHeight="12500" activeTab="2" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1650,7 +1651,8 @@
   <dimension ref="A1:CR54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
func print_tabzeile neu: eine Zeile printen report_home: wie report_send_Move
0xAD: abschnittnummer > 0 abfragen: Error bei send_move, home

l 5319:  letzten Punkt fuellen

Platteview:
markfeldarray.last füllen
l 485:
</commit_message>
<xml_diff>
--- a/CNC_Mill/Daten Lage.xlsx
+++ b/CNC_Mill/Daten Lage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/CNC-Projekt/CNC_Mill/CNC_Mill/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4AE1FB-60CB-8B4B-BBED-1340B4894D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD10FF2B-DF81-5A45-AFDE-722A7FF595DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="13040" windowWidth="37240" windowHeight="12500" activeTab="2" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
+    <workbookView xWindow="5380" yWindow="7120" windowWidth="37240" windowHeight="12500" activeTab="2" xr2:uid="{4D2B1F18-4B43-A146-B674-6FCE3AF3D0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1651,8 +1650,8 @@
   <dimension ref="A1:CR54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <pane ySplit="3" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2372,354 +2371,1026 @@
       <c r="AV8" s="5"/>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
-      <c r="AG10" s="5"/>
-      <c r="AH10" s="5"/>
-      <c r="AI10" s="5"/>
-      <c r="AJ10" s="5"/>
-      <c r="AK10" s="5"/>
-      <c r="AL10" s="5"/>
-      <c r="AM10" s="5"/>
-      <c r="AN10" s="5"/>
-      <c r="AO10" s="5"/>
-      <c r="AP10" s="5"/>
-      <c r="AQ10" s="5"/>
-      <c r="AR10" s="5"/>
-      <c r="AS10" s="5"/>
-      <c r="AT10" s="5"/>
-      <c r="AU10" s="5"/>
-      <c r="AV10" s="5"/>
+      <c r="A10" s="5">
+        <v>102</v>
+      </c>
+      <c r="B10" s="5">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>61</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>213</v>
+      </c>
+      <c r="J10" s="5">
+        <v>4</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
+        <v>128</v>
+      </c>
+      <c r="M10" s="5">
+        <v>157</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="5">
+        <v>2</v>
+      </c>
+      <c r="P10" s="5">
+        <v>128</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="5">
+        <v>0</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+      <c r="W10" s="5">
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>77</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>10</v>
+      </c>
+      <c r="AF10" s="5">
+        <v>128</v>
+      </c>
+      <c r="AG10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="5">
+        <v>255</v>
+      </c>
+      <c r="AM10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="5">
+        <v>255</v>
+      </c>
+      <c r="AQ10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AR10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="17"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="17"/>
-      <c r="V11" s="17"/>
-      <c r="W11" s="17"/>
-      <c r="X11" s="17"/>
-      <c r="Y11" s="17"/>
-      <c r="Z11" s="17"/>
-      <c r="AA11" s="17"/>
-      <c r="AB11" s="17"/>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="17"/>
-      <c r="AH11" s="17"/>
-      <c r="AI11" s="17"/>
-      <c r="AJ11" s="17"/>
-      <c r="AK11" s="17"/>
-      <c r="AL11" s="17"/>
-      <c r="AM11" s="17"/>
-      <c r="AN11" s="17"/>
-      <c r="AO11" s="17"/>
-      <c r="AP11" s="17"/>
-      <c r="AQ11" s="17"/>
-      <c r="AR11" s="17"/>
-      <c r="AS11" s="17"/>
-      <c r="AT11" s="17"/>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="17"/>
+      <c r="A11" s="17">
+        <v>0</v>
+      </c>
+      <c r="B11" s="17">
+        <v>0</v>
+      </c>
+      <c r="C11" s="17">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17">
+        <v>0</v>
+      </c>
+      <c r="E11" s="17">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
+      <c r="H11" s="17">
+        <v>0</v>
+      </c>
+      <c r="I11" s="17">
+        <v>0</v>
+      </c>
+      <c r="J11" s="17">
+        <v>0</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="17">
+        <v>0</v>
+      </c>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>64</v>
+      </c>
+      <c r="R11" s="17">
+        <v>6</v>
+      </c>
+      <c r="S11" s="17">
+        <v>0</v>
+      </c>
+      <c r="T11" s="17">
+        <v>128</v>
+      </c>
+      <c r="U11" s="17">
+        <v>0</v>
+      </c>
+      <c r="V11" s="17">
+        <v>0</v>
+      </c>
+      <c r="W11" s="17">
+        <v>0</v>
+      </c>
+      <c r="X11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC11" s="17">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="17">
+        <v>77</v>
+      </c>
+      <c r="AE11" s="17">
+        <v>10</v>
+      </c>
+      <c r="AF11" s="17">
+        <v>128</v>
+      </c>
+      <c r="AG11" s="17">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="17">
+        <v>255</v>
+      </c>
+      <c r="AM11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AN11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AQ11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AT11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="8"/>
-      <c r="AB12" s="8"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="8"/>
-      <c r="AE12" s="8"/>
-      <c r="AF12" s="8"/>
-      <c r="AG12" s="8"/>
-      <c r="AH12" s="8"/>
-      <c r="AI12" s="8"/>
-      <c r="AJ12" s="8"/>
-      <c r="AK12" s="8"/>
-      <c r="AL12" s="8"/>
-      <c r="AM12" s="8"/>
-      <c r="AN12" s="8"/>
-      <c r="AO12" s="8"/>
-      <c r="AP12" s="8"/>
-      <c r="AQ12" s="8"/>
-      <c r="AR12" s="8"/>
-      <c r="AS12" s="8"/>
-      <c r="AT12" s="8"/>
-      <c r="AU12" s="8"/>
-      <c r="AV12" s="8"/>
+      <c r="A12" s="8">
+        <v>0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>0</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>64</v>
+      </c>
+      <c r="R12" s="8">
+        <v>6</v>
+      </c>
+      <c r="S12" s="8">
+        <v>0</v>
+      </c>
+      <c r="T12" s="8">
+        <v>128</v>
+      </c>
+      <c r="U12" s="8">
+        <v>0</v>
+      </c>
+      <c r="V12" s="8">
+        <v>0</v>
+      </c>
+      <c r="W12" s="8">
+        <v>0</v>
+      </c>
+      <c r="X12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD12" s="8">
+        <v>77</v>
+      </c>
+      <c r="AE12" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF12" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG12" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="8">
+        <v>255</v>
+      </c>
+      <c r="AM12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU12" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV12" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8"/>
-      <c r="V13" s="8"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="15"/>
-      <c r="AA13" s="8"/>
-      <c r="AB13" s="8"/>
-      <c r="AC13" s="8"/>
-      <c r="AD13" s="8"/>
-      <c r="AE13" s="8"/>
-      <c r="AF13" s="8"/>
-      <c r="AG13" s="8"/>
-      <c r="AH13" s="8"/>
-      <c r="AI13" s="8"/>
-      <c r="AJ13" s="8"/>
-      <c r="AK13" s="8"/>
-      <c r="AL13" s="8"/>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="8"/>
-      <c r="AO13" s="8"/>
-      <c r="AP13" s="8"/>
-      <c r="AQ13" s="8"/>
-      <c r="AR13" s="8"/>
-      <c r="AS13" s="8"/>
-      <c r="AT13" s="8"/>
-      <c r="AU13" s="8"/>
-      <c r="AV13" s="8"/>
+      <c r="A13" s="8">
+        <v>0</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>64</v>
+      </c>
+      <c r="R13" s="8">
+        <v>6</v>
+      </c>
+      <c r="S13" s="8">
+        <v>0</v>
+      </c>
+      <c r="T13" s="8">
+        <v>0</v>
+      </c>
+      <c r="U13" s="8">
+        <v>0</v>
+      </c>
+      <c r="V13" s="8">
+        <v>0</v>
+      </c>
+      <c r="W13" s="8">
+        <v>0</v>
+      </c>
+      <c r="X13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>77</v>
+      </c>
+      <c r="AE13" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF13" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="8">
+        <v>255</v>
+      </c>
+      <c r="AM13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV13" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="8"/>
-      <c r="AB14" s="8"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-      <c r="AF14" s="8"/>
-      <c r="AG14" s="8"/>
-      <c r="AH14" s="8"/>
-      <c r="AI14" s="8"/>
-      <c r="AJ14" s="8"/>
-      <c r="AK14" s="8"/>
-      <c r="AL14" s="8"/>
-      <c r="AM14" s="8"/>
-      <c r="AN14" s="8"/>
-      <c r="AO14" s="8"/>
-      <c r="AP14" s="8"/>
-      <c r="AQ14" s="8"/>
-      <c r="AR14" s="8"/>
-      <c r="AS14" s="8"/>
-      <c r="AT14" s="8"/>
-      <c r="AU14" s="8"/>
-      <c r="AV14" s="8"/>
+      <c r="A14" s="8">
+        <v>198</v>
+      </c>
+      <c r="B14" s="8">
+        <v>2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>171</v>
+      </c>
+      <c r="J14" s="8">
+        <v>12</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>58</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>4</v>
+      </c>
+      <c r="P14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0</v>
+      </c>
+      <c r="S14" s="8">
+        <v>0</v>
+      </c>
+      <c r="T14" s="8">
+        <v>0</v>
+      </c>
+      <c r="U14" s="8">
+        <v>0</v>
+      </c>
+      <c r="V14" s="8">
+        <v>0</v>
+      </c>
+      <c r="W14" s="8">
+        <v>0</v>
+      </c>
+      <c r="X14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>4</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>2</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>77</v>
+      </c>
+      <c r="AE14" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF14" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="8">
+        <v>255</v>
+      </c>
+      <c r="AM14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="8">
+        <v>255</v>
+      </c>
+      <c r="AQ14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AR14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV14" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="8"/>
-      <c r="AB15" s="8"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-      <c r="AF15" s="8"/>
-      <c r="AG15" s="8"/>
-      <c r="AH15" s="8"/>
-      <c r="AI15" s="8"/>
-      <c r="AJ15" s="8"/>
-      <c r="AK15" s="8"/>
-      <c r="AL15" s="8"/>
-      <c r="AM15" s="8"/>
-      <c r="AN15" s="8"/>
-      <c r="AO15" s="8"/>
-      <c r="AP15" s="8"/>
-      <c r="AQ15" s="8"/>
-      <c r="AR15" s="8"/>
-      <c r="AS15" s="8"/>
-      <c r="AT15" s="8"/>
-      <c r="AU15" s="8"/>
-      <c r="AV15" s="8"/>
+      <c r="A15" s="8">
+        <v>0</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="8">
+        <v>0</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>0</v>
+      </c>
+      <c r="N15" s="8">
+        <v>0</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>64</v>
+      </c>
+      <c r="R15" s="8">
+        <v>6</v>
+      </c>
+      <c r="S15" s="8">
+        <v>0</v>
+      </c>
+      <c r="T15" s="8">
+        <v>128</v>
+      </c>
+      <c r="U15" s="8">
+        <v>0</v>
+      </c>
+      <c r="V15" s="8">
+        <v>0</v>
+      </c>
+      <c r="W15" s="8">
+        <v>0</v>
+      </c>
+      <c r="X15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="8">
+        <v>5</v>
+      </c>
+      <c r="AC15" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="8">
+        <v>77</v>
+      </c>
+      <c r="AE15" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF15" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG15" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="8">
+        <v>255</v>
+      </c>
+      <c r="AM15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="8">
+        <v>1</v>
+      </c>
+      <c r="AR15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:96" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="8"/>
-      <c r="AB16" s="8"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-      <c r="AF16" s="8"/>
-      <c r="AG16" s="8"/>
-      <c r="AH16" s="8"/>
-      <c r="AI16" s="8"/>
-      <c r="AJ16" s="8"/>
-      <c r="AK16" s="8"/>
-      <c r="AL16" s="8"/>
-      <c r="AM16" s="8"/>
-      <c r="AN16" s="8"/>
-      <c r="AO16" s="8"/>
-      <c r="AP16" s="8"/>
-      <c r="AQ16" s="8"/>
-      <c r="AR16" s="8"/>
-      <c r="AS16" s="8"/>
-      <c r="AT16" s="8"/>
-      <c r="AU16" s="8"/>
-      <c r="AV16" s="8"/>
+      <c r="A16" s="8">
+        <v>0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0</v>
+      </c>
+      <c r="N16" s="8">
+        <v>0</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>64</v>
+      </c>
+      <c r="R16" s="8">
+        <v>6</v>
+      </c>
+      <c r="S16" s="8">
+        <v>0</v>
+      </c>
+      <c r="T16" s="8">
+        <v>0</v>
+      </c>
+      <c r="U16" s="8">
+        <v>0</v>
+      </c>
+      <c r="V16" s="8">
+        <v>0</v>
+      </c>
+      <c r="W16" s="8">
+        <v>0</v>
+      </c>
+      <c r="X16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="8">
+        <v>6</v>
+      </c>
+      <c r="AC16" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD16" s="8">
+        <v>77</v>
+      </c>
+      <c r="AE16" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF16" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="8">
+        <v>255</v>
+      </c>
+      <c r="AM16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU16" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV16" s="8">
+        <v>0</v>
+      </c>
       <c r="AX16" s="12"/>
       <c r="AY16" s="12"/>
       <c r="AZ16" s="12"/>
@@ -2769,57 +3440,153 @@
       <c r="CR16" s="12"/>
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="15"/>
-      <c r="AA17" s="8"/>
-      <c r="AB17" s="8"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-      <c r="AF17" s="8"/>
-      <c r="AG17" s="8"/>
-      <c r="AH17" s="8"/>
-      <c r="AI17" s="8"/>
-      <c r="AJ17" s="8"/>
-      <c r="AK17" s="8"/>
-      <c r="AL17" s="8"/>
-      <c r="AM17" s="8"/>
-      <c r="AN17" s="8"/>
-      <c r="AO17" s="8"/>
-      <c r="AP17" s="8"/>
-      <c r="AQ17" s="8"/>
-      <c r="AR17" s="8"/>
-      <c r="AS17" s="8"/>
-      <c r="AT17" s="8"/>
-      <c r="AU17" s="8"/>
-      <c r="AV17" s="8"/>
+      <c r="A17" s="8">
+        <v>0</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>0</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0</v>
+      </c>
+      <c r="P17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>64</v>
+      </c>
+      <c r="R17" s="8">
+        <v>6</v>
+      </c>
+      <c r="S17" s="8">
+        <v>0</v>
+      </c>
+      <c r="T17" s="8">
+        <v>0</v>
+      </c>
+      <c r="U17" s="8">
+        <v>0</v>
+      </c>
+      <c r="V17" s="8">
+        <v>0</v>
+      </c>
+      <c r="W17" s="8">
+        <v>0</v>
+      </c>
+      <c r="X17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="8">
+        <v>7</v>
+      </c>
+      <c r="AC17" s="8">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="8">
+        <v>77</v>
+      </c>
+      <c r="AE17" s="8">
+        <v>10</v>
+      </c>
+      <c r="AF17" s="8">
+        <v>128</v>
+      </c>
+      <c r="AG17" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="8">
+        <v>255</v>
+      </c>
+      <c r="AM17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO17" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ17" s="8">
+        <v>1</v>
+      </c>
+      <c r="AR17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU17" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV17" s="8">
+        <v>0</v>
+      </c>
       <c r="AW17" s="8"/>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -2870,296 +3637,104 @@
       <c r="AV18" s="8"/>
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A19" s="8">
-        <v>0</v>
-      </c>
-      <c r="B19" s="8">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="F19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="8">
-        <v>0</v>
-      </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="I19" s="8">
-        <v>0</v>
-      </c>
-      <c r="J19" s="8">
-        <v>0</v>
-      </c>
-      <c r="K19" s="8">
-        <v>0</v>
-      </c>
-      <c r="L19" s="8">
-        <v>0</v>
-      </c>
-      <c r="M19" s="8">
-        <v>0</v>
-      </c>
-      <c r="N19" s="8">
-        <v>0</v>
-      </c>
-      <c r="O19" s="8">
-        <v>0</v>
-      </c>
-      <c r="P19" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="8">
-        <v>131</v>
-      </c>
-      <c r="R19" s="8">
-        <v>5</v>
-      </c>
-      <c r="S19" s="8">
-        <v>0</v>
-      </c>
-      <c r="T19" s="8">
-        <v>128</v>
-      </c>
-      <c r="U19" s="8">
-        <v>0</v>
-      </c>
-      <c r="V19" s="8">
-        <v>0</v>
-      </c>
-      <c r="W19" s="8">
-        <v>0</v>
-      </c>
-      <c r="X19" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="15">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="8">
-        <v>4</v>
-      </c>
-      <c r="AD19" s="8">
-        <v>128</v>
-      </c>
-      <c r="AE19" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF19" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL19" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU19" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV19" s="8">
-        <v>0</v>
-      </c>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8"/>
+      <c r="AH19" s="8"/>
+      <c r="AI19" s="8"/>
+      <c r="AJ19" s="8"/>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
+      <c r="AM19" s="8"/>
+      <c r="AN19" s="8"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="8"/>
+      <c r="AR19" s="8"/>
+      <c r="AS19" s="8"/>
+      <c r="AT19" s="8"/>
+      <c r="AU19" s="8"/>
+      <c r="AV19" s="8"/>
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A20" s="8">
-        <v>0</v>
-      </c>
-      <c r="B20" s="8">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8">
-        <v>0</v>
-      </c>
-      <c r="D20" s="8">
-        <v>0</v>
-      </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-      <c r="F20" s="8">
-        <v>0</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0</v>
-      </c>
-      <c r="I20" s="8">
-        <v>0</v>
-      </c>
-      <c r="J20" s="8">
-        <v>0</v>
-      </c>
-      <c r="K20" s="8">
-        <v>0</v>
-      </c>
-      <c r="L20" s="8">
-        <v>0</v>
-      </c>
-      <c r="M20" s="8">
-        <v>0</v>
-      </c>
-      <c r="N20" s="8">
-        <v>0</v>
-      </c>
-      <c r="O20" s="8">
-        <v>0</v>
-      </c>
-      <c r="P20" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="8">
-        <v>131</v>
-      </c>
-      <c r="R20" s="8">
-        <v>5</v>
-      </c>
-      <c r="S20" s="8">
-        <v>0</v>
-      </c>
-      <c r="T20" s="8">
-        <v>0</v>
-      </c>
-      <c r="U20" s="8">
-        <v>0</v>
-      </c>
-      <c r="V20" s="8">
-        <v>0</v>
-      </c>
-      <c r="W20" s="8">
-        <v>0</v>
-      </c>
-      <c r="X20" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="15">
-        <v>2</v>
-      </c>
-      <c r="AA20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="8">
-        <v>1</v>
-      </c>
-      <c r="AC20" s="8">
-        <v>4</v>
-      </c>
-      <c r="AD20" s="8">
-        <v>64</v>
-      </c>
-      <c r="AE20" s="8">
-        <v>10</v>
-      </c>
-      <c r="AF20" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG20" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL20" s="8">
-        <v>255</v>
-      </c>
-      <c r="AM20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU20" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV20" s="8">
-        <v>0</v>
-      </c>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="8"/>
+      <c r="AT20" s="8"/>
+      <c r="AU20" s="8"/>
+      <c r="AV20" s="8"/>
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
@@ -3262,296 +3837,104 @@
       <c r="AV22" s="8"/>
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A23" s="8">
-        <v>0</v>
-      </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0</v>
-      </c>
-      <c r="E23" s="8">
-        <v>0</v>
-      </c>
-      <c r="F23" s="8">
-        <v>0</v>
-      </c>
-      <c r="G23" s="8">
-        <v>0</v>
-      </c>
-      <c r="H23" s="8">
-        <v>0</v>
-      </c>
-      <c r="I23" s="8">
-        <v>0</v>
-      </c>
-      <c r="J23" s="8">
-        <v>0</v>
-      </c>
-      <c r="K23" s="8">
-        <v>0</v>
-      </c>
-      <c r="L23" s="8">
-        <v>0</v>
-      </c>
-      <c r="M23" s="8">
-        <v>0</v>
-      </c>
-      <c r="N23" s="8">
-        <v>0</v>
-      </c>
-      <c r="O23" s="8">
-        <v>0</v>
-      </c>
-      <c r="P23" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="8">
-        <v>228</v>
-      </c>
-      <c r="R23" s="8">
-        <v>6</v>
-      </c>
-      <c r="S23" s="8">
-        <v>0</v>
-      </c>
-      <c r="T23" s="8">
-        <v>128</v>
-      </c>
-      <c r="U23" s="8">
-        <v>0</v>
-      </c>
-      <c r="V23" s="8">
-        <v>0</v>
-      </c>
-      <c r="W23" s="8">
-        <v>0</v>
-      </c>
-      <c r="X23" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y23" s="8">
-        <v>186</v>
-      </c>
-      <c r="Z23" s="15">
-        <v>3</v>
-      </c>
-      <c r="AA23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="8">
-        <v>4</v>
-      </c>
-      <c r="AD23" s="8">
-        <v>99</v>
-      </c>
-      <c r="AE23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF23" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG23" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM23" s="8">
-        <v>24</v>
-      </c>
-      <c r="AN23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU23" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV23" s="8">
-        <v>0</v>
-      </c>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8"/>
+      <c r="AN23" s="8"/>
+      <c r="AO23" s="8"/>
+      <c r="AP23" s="8"/>
+      <c r="AQ23" s="8"/>
+      <c r="AR23" s="8"/>
+      <c r="AS23" s="8"/>
+      <c r="AT23" s="8"/>
+      <c r="AU23" s="8"/>
+      <c r="AV23" s="8"/>
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.2">
-      <c r="A24" s="8">
-        <v>0</v>
-      </c>
-      <c r="B24" s="8">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8">
-        <v>0</v>
-      </c>
-      <c r="D24" s="8">
-        <v>0</v>
-      </c>
-      <c r="E24" s="8">
-        <v>0</v>
-      </c>
-      <c r="F24" s="8">
-        <v>0</v>
-      </c>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0</v>
-      </c>
-      <c r="I24" s="8">
-        <v>0</v>
-      </c>
-      <c r="J24" s="8">
-        <v>0</v>
-      </c>
-      <c r="K24" s="8">
-        <v>0</v>
-      </c>
-      <c r="L24" s="8">
-        <v>0</v>
-      </c>
-      <c r="M24" s="8">
-        <v>0</v>
-      </c>
-      <c r="N24" s="8">
-        <v>0</v>
-      </c>
-      <c r="O24" s="8">
-        <v>0</v>
-      </c>
-      <c r="P24" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="8">
-        <v>228</v>
-      </c>
-      <c r="R24" s="8">
-        <v>6</v>
-      </c>
-      <c r="S24" s="8">
-        <v>0</v>
-      </c>
-      <c r="T24" s="8">
-        <v>128</v>
-      </c>
-      <c r="U24" s="8">
-        <v>0</v>
-      </c>
-      <c r="V24" s="8">
-        <v>0</v>
-      </c>
-      <c r="W24" s="8">
-        <v>0</v>
-      </c>
-      <c r="X24" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="8">
-        <v>186</v>
-      </c>
-      <c r="Z24" s="15">
-        <v>3</v>
-      </c>
-      <c r="AA24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="8">
-        <v>4</v>
-      </c>
-      <c r="AD24" s="8">
-        <v>99</v>
-      </c>
-      <c r="AE24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="8">
-        <v>128</v>
-      </c>
-      <c r="AG24" s="8">
-        <v>1</v>
-      </c>
-      <c r="AH24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="8">
-        <v>24</v>
-      </c>
-      <c r="AN24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU24" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV24" s="8">
-        <v>0</v>
-      </c>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
+      <c r="AN24" s="8"/>
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="8"/>
+      <c r="AQ24" s="8"/>
+      <c r="AR24" s="8"/>
+      <c r="AS24" s="8"/>
+      <c r="AT24" s="8"/>
+      <c r="AU24" s="8"/>
+      <c r="AV24" s="8"/>
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A25" s="8"/>

</xml_diff>